<commit_message>
update on sprint1 CUST feature + Customer.java
</commit_message>
<xml_diff>
--- a/P05/Scrum.xlsx
+++ b/P05/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11162A06-F9F2-1748-B128-2996150BB04E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4C8F21-C166-DD4B-BE58-E8AFBF0F360C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="146">
   <si>
     <t>Product Name:</t>
   </si>
@@ -477,6 +477,9 @@
   </si>
   <si>
     <t>In Work</t>
+  </si>
+  <si>
+    <t>Completed Day 5</t>
   </si>
 </sst>
 </file>
@@ -1302,13 +1305,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3663,7 +3666,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -5417,8 +5420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5608,11 +5611,11 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -5626,7 +5629,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5644,7 +5647,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5697,7 +5700,9 @@
       <c r="D17" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -5711,7 +5716,9 @@
       <c r="D18" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="E18" s="37"/>
+      <c r="E18" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="F18" s="38"/>
     </row>
     <row r="19" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -5725,7 +5732,9 @@
       <c r="D19" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="E19" s="37"/>
+      <c r="E19" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
update on scrum product backlog
</commit_message>
<xml_diff>
--- a/P05/Scrum.xlsx
+++ b/P05/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4C8F21-C166-DD4B-BE58-E8AFBF0F360C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948E5745-3213-524E-8159-8F8BBF8ED114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="147">
   <si>
     <t>Product Name:</t>
   </si>
@@ -470,16 +470,19 @@
     <t>Copy build.xml + git push Customer.java to repo</t>
   </si>
   <si>
-    <t>Make sure the data validation works correctly</t>
-  </si>
-  <si>
-    <t>Write the Option class, has Inheritance</t>
-  </si>
-  <si>
     <t>In Work</t>
   </si>
   <si>
     <t>Completed Day 5</t>
+  </si>
+  <si>
+    <t>push Option.java to repo</t>
+  </si>
+  <si>
+    <t>In Test</t>
+  </si>
+  <si>
+    <t>Write the Option class, following the UML Diagram</t>
   </si>
 </sst>
 </file>
@@ -1840,7 +1843,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -1989,7 +1992,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -2063,7 +2066,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -2782,7 +2785,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -2931,7 +2934,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -3005,7 +3008,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3666,8 +3669,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4102,7 +4105,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H24" s="18" t="s">
         <v>31</v>
@@ -4135,7 +4138,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>36</v>
@@ -5420,8 +5423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5701,7 +5704,7 @@
         <v>139</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F17" s="38"/>
     </row>
@@ -5717,7 +5720,7 @@
         <v>140</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F18" s="38"/>
     </row>
@@ -5733,7 +5736,7 @@
         <v>141</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F19" s="38"/>
     </row>
@@ -5746,7 +5749,7 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="39" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E20" s="37"/>
       <c r="F20" s="38"/>
@@ -5774,7 +5777,7 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="39" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E22" s="37"/>
       <c r="F22" s="38"/>
@@ -6616,7 +6619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated scrum + Option.java
</commit_message>
<xml_diff>
--- a/P05/Scrum.xlsx
+++ b/P05/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948E5745-3213-524E-8159-8F8BBF8ED114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDCA43C-584A-2B49-B6E5-D17AF2669F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="147">
   <si>
     <t>Product Name:</t>
   </si>
@@ -1308,13 +1308,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3669,7 +3669,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -5424,7 +5424,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5614,11 +5614,11 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -5632,7 +5632,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5650,7 +5650,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5751,7 +5751,9 @@
       <c r="D20" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="E20" s="37"/>
+      <c r="E20" s="37" t="s">
+        <v>143</v>
+      </c>
       <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -5765,7 +5767,9 @@
       <c r="D21" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="37"/>
+      <c r="E21" s="37" t="s">
+        <v>143</v>
+      </c>
       <c r="F21" s="38"/>
     </row>
     <row r="22" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -5779,7 +5783,9 @@
       <c r="D22" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="37"/>
+      <c r="E22" s="37" t="s">
+        <v>143</v>
+      </c>
       <c r="F22" s="38"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
update on scrum sprint1 tasks
</commit_message>
<xml_diff>
--- a/P05/Scrum.xlsx
+++ b/P05/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDCA43C-584A-2B49-B6E5-D17AF2669F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAF9390-C85E-F34F-AF5A-D3CB6CD633E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="151">
   <si>
     <t>Product Name:</t>
   </si>
@@ -483,6 +483,18 @@
   </si>
   <si>
     <t>Write the Option class, following the UML Diagram</t>
+  </si>
+  <si>
+    <t>Write Computer Class, following the UML Diagram</t>
+  </si>
+  <si>
+    <t>implement the ArrayList of Option</t>
+  </si>
+  <si>
+    <t>Write the Order class, following the UML Diagram</t>
+  </si>
+  <si>
+    <t>implement the ArrayList of Computer</t>
   </si>
 </sst>
 </file>
@@ -1293,28 +1305,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="6">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="7">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3669,8 +3681,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3711,7 +3723,9 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="44">
+        <v>243</v>
+      </c>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
@@ -4138,7 +4152,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>36</v>
@@ -4170,7 +4184,9 @@
       <c r="F26" s="17">
         <v>1</v>
       </c>
-      <c r="G26" s="17"/>
+      <c r="G26" s="17" t="s">
+        <v>142</v>
+      </c>
       <c r="H26" s="18" t="s">
         <v>31</v>
       </c>
@@ -4199,7 +4215,9 @@
       <c r="F27" s="17">
         <v>1</v>
       </c>
-      <c r="G27" s="17"/>
+      <c r="G27" s="17" t="s">
+        <v>142</v>
+      </c>
       <c r="H27" s="18" t="s">
         <v>31</v>
       </c>
@@ -5423,8 +5441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5527,7 +5545,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5542,7 +5560,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5560,7 +5578,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5578,7 +5596,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5596,7 +5614,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5614,7 +5632,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5632,7 +5650,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5650,7 +5668,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5788,64 +5806,100 @@
       </c>
       <c r="F22" s="38"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="37"/>
+      <c r="D23" s="39" t="s">
+        <v>147</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>142</v>
+      </c>
       <c r="F23" s="38"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="37"/>
+      <c r="D24" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>142</v>
+      </c>
       <c r="F24" s="38"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="37"/>
+      <c r="D25" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>142</v>
+      </c>
       <c r="F25" s="38"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="4">
         <v>10</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="37"/>
+      <c r="D26" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>142</v>
+      </c>
       <c r="F26" s="38"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="4">
         <v>11</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="37"/>
+      <c r="D27" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>142</v>
+      </c>
       <c r="F27" s="38"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="4">
         <v>12</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="37"/>
+      <c r="D28" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>142</v>
+      </c>
       <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Computer.java + updates in scrum
</commit_message>
<xml_diff>
--- a/P05/Scrum.xlsx
+++ b/P05/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAF9390-C85E-F34F-AF5A-D3CB6CD633E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CE85BF-C101-F64F-836A-B2908BC0EB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -1320,13 +1320,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3681,8 +3681,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4185,7 +4185,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H26" s="18" t="s">
         <v>31</v>
@@ -5441,8 +5441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5632,11 +5632,11 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -5650,7 +5650,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5668,7 +5668,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5818,7 +5818,7 @@
         <v>147</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F23" s="38"/>
     </row>
@@ -5834,7 +5834,7 @@
         <v>140</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F24" s="38"/>
     </row>
@@ -5850,7 +5850,7 @@
         <v>148</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F25" s="38"/>
     </row>

</xml_diff>

<commit_message>
order.java + scrum update + modif on equals method of past classes
</commit_message>
<xml_diff>
--- a/P05/Scrum.xlsx
+++ b/P05/Scrum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CE85BF-C101-F64F-836A-B2908BC0EB0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985ECADB-4EDF-5A4E-AF48-6582017A1FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="150">
   <si>
     <t>Product Name:</t>
   </si>
@@ -468,9 +468,6 @@
   </si>
   <si>
     <t>Copy build.xml + git push Customer.java to repo</t>
-  </si>
-  <si>
-    <t>In Work</t>
   </si>
   <si>
     <t>Completed Day 5</t>
@@ -1320,13 +1317,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3682,7 +3679,7 @@
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4119,7 +4116,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H24" s="18" t="s">
         <v>31</v>
@@ -4152,7 +4149,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>36</v>
@@ -4185,7 +4182,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H26" s="18" t="s">
         <v>31</v>
@@ -4216,7 +4213,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H27" s="18" t="s">
         <v>31</v>
@@ -4246,7 +4243,9 @@
       <c r="F28" s="17">
         <v>1</v>
       </c>
-      <c r="G28" s="17"/>
+      <c r="G28" s="17" t="s">
+        <v>144</v>
+      </c>
       <c r="H28" s="18" t="s">
         <v>31</v>
       </c>
@@ -5441,8 +5440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5632,11 +5631,11 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -5650,7 +5649,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5668,7 +5667,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5722,7 +5721,7 @@
         <v>139</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F17" s="38"/>
     </row>
@@ -5738,7 +5737,7 @@
         <v>140</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F18" s="38"/>
     </row>
@@ -5754,7 +5753,7 @@
         <v>141</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F19" s="38"/>
     </row>
@@ -5767,10 +5766,10 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F20" s="38"/>
     </row>
@@ -5786,7 +5785,7 @@
         <v>140</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F21" s="38"/>
     </row>
@@ -5799,10 +5798,10 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F22" s="38"/>
     </row>
@@ -5815,10 +5814,10 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E23" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F23" s="38"/>
     </row>
@@ -5834,7 +5833,7 @@
         <v>140</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F24" s="38"/>
     </row>
@@ -5847,10 +5846,10 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F25" s="38"/>
     </row>
@@ -5863,7 +5862,7 @@
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E26" s="37" t="s">
         <v>142</v>
@@ -5895,7 +5894,7 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E28" s="37" t="s">
         <v>142</v>

</xml_diff>

<commit_message>
final scrum for sprint1
</commit_message>
<xml_diff>
--- a/P05/Scrum.xlsx
+++ b/P05/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985ECADB-4EDF-5A4E-AF48-6582017A1FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69590FE9-E2B6-7043-846D-FC7AECC2FA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -476,9 +476,6 @@
     <t>push Option.java to repo</t>
   </si>
   <si>
-    <t>In Test</t>
-  </si>
-  <si>
     <t>Write the Option class, following the UML Diagram</t>
   </si>
   <si>
@@ -492,6 +489,9 @@
   </si>
   <si>
     <t>implement the ArrayList of Computer</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 1</t>
   </si>
 </sst>
 </file>
@@ -1005,19 +1005,19 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3678,7 +3678,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -3889,11 +3889,11 @@
       </c>
       <c r="B13" s="5">
         <f>B12-C13</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C13" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 1")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="5"/>
@@ -3913,7 +3913,7 @@
       </c>
       <c r="B14" s="5">
         <f>B13-C14</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C14" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 2")</f>
@@ -3937,7 +3937,7 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 3")</f>
@@ -3961,7 +3961,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -4116,7 +4116,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H24" s="18" t="s">
         <v>31</v>
@@ -4149,7 +4149,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>36</v>
@@ -4182,7 +4182,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H26" s="18" t="s">
         <v>31</v>
@@ -4213,7 +4213,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H27" s="18" t="s">
         <v>31</v>
@@ -4244,7 +4244,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H28" s="18" t="s">
         <v>31</v>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E20" s="37" t="s">
         <v>142</v>
@@ -5814,7 +5814,7 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>142</v>
@@ -5846,7 +5846,7 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E25" s="37" t="s">
         <v>142</v>
@@ -5862,7 +5862,7 @@
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="39" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E26" s="37" t="s">
         <v>142</v>
@@ -5894,7 +5894,7 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E28" s="37" t="s">
         <v>142</v>

</xml_diff>